<commit_message>
Version with improved filtering mechanism among divsRetreived
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B1B90D2-44D7-4887-B342-D7A50E252C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865C5719-91D7-4EB9-8513-3BA35ECCE731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing phase 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Page</t>
   </si>
@@ -84,6 +85,9 @@
   </si>
   <si>
     <t>https://www.blazemeter.com/blog/import-lodash-libraries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -107,12 +111,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,9 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,6 +488,229 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D388E1-07C2-4438-87C9-DFEAF3624581}">
   <dimension ref="A2:E14"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1192</v>
+      </c>
+      <c r="E8">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>235</v>
+      </c>
+      <c r="E9">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>202</v>
+      </c>
+      <c r="E10">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>64</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
+    <sortCondition ref="C1:C14"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{98A2431F-4D0A-4572-90A4-2E51F9447E35}"/>
+    <hyperlink ref="B9" r:id="rId2" location="6468" xr:uid="{111B0D08-DC1A-4DBB-9ECC-C5F270836E4E}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{624940F1-567F-42ED-B197-B88202746E43}"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{B969220C-FF2B-4DB1-83F4-547C43F1AE38}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{6C9DC17C-150E-472F-B8E6-04B55FA192C5}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{5967D9D2-A865-4C38-8954-B6BE51989855}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{9533B587-ACE8-48EE-A7F8-81EB68A08C2B}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{324FA744-A239-4D81-8343-6B0B787B9372}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{28BD90B5-F257-4550-B1C1-B4DC060B4276}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{93B637F0-C5FB-4481-8DF5-01028855AF2F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6537F556-4FCE-4387-B0A5-42EE745AE473}">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
@@ -495,27 +738,21 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1192</v>
-      </c>
-      <c r="E3">
-        <v>2560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -523,21 +760,27 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>76</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2560</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -545,33 +788,33 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>235</v>
-      </c>
-      <c r="E7">
-        <v>2560</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>839</v>
+      </c>
+      <c r="E7" s="5">
+        <v>660</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>202</v>
+        <v>1192</v>
       </c>
       <c r="E8">
         <v>2560</v>
@@ -579,124 +822,124 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>235</v>
+      </c>
+      <c r="E9" s="3">
         <v>2560</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>78</v>
-      </c>
-      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>202</v>
+      </c>
+      <c r="E10" s="3">
         <v>2560</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>226</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2048</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>64</v>
-      </c>
-      <c r="E14">
-        <v>64</v>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>276</v>
+      </c>
+      <c r="E14" s="5">
+        <v>650</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{98A2431F-4D0A-4572-90A4-2E51F9447E35}"/>
-    <hyperlink ref="B7" r:id="rId2" location="6468" xr:uid="{111B0D08-DC1A-4DBB-9ECC-C5F270836E4E}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{624940F1-567F-42ED-B197-B88202746E43}"/>
-    <hyperlink ref="B9" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{B969220C-FF2B-4DB1-83F4-547C43F1AE38}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{6C9DC17C-150E-472F-B8E6-04B55FA192C5}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{04BB8B05-693A-43D5-8AC1-5BF9FD42F37A}"/>
+    <hyperlink ref="B9" r:id="rId2" location="6468" xr:uid="{12630F07-19E6-401D-915A-54C60485D558}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{129B6192-072A-46E6-867E-9C15C240DD49}"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{B0A92007-36D3-4FB4-BC35-3671D2485743}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{A4EECCB2-7321-4BA5-8EE5-A3525FE51F3B}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{E9A2C33E-F64B-46D3-BAD1-3B2C91ACA23C}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{DD788729-1CA6-48F2-9A6A-B6227A30CEB1}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{ED30A7AF-0FDC-4C2E-83F4-29491714F2B6}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{CF801DD5-0FC2-4107-92D0-BD6B62BDF78E}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{03D017B3-D6E5-4671-B253-C3D0888C7EBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a631a279-5a15-4d42-8c5c-c081a45901f6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -923,32 +1166,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB8DB88-F110-4C4D-B0CC-7321E21A6D86}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f8a1abd1-0732-4ba5-993c-eb9e15cff616"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a631a279-5a15-4d42-8c5c-c081a45901f6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -965,4 +1200,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB8DB88-F110-4C4D-B0CC-7321E21A6D86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f8a1abd1-0732-4ba5-993c-eb9e15cff616"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
use webpak to imprt lodash
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865C5719-91D7-4EB9-8513-3BA35ECCE731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E261F-056B-41ED-A21F-2094B0653991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
     <sheet name="Testing phase 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Testing phase 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
   <si>
     <t>Page</t>
   </si>
@@ -88,6 +90,120 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>No results because there is a big div and inside of it we should look for info</t>
+  </si>
+  <si>
+    <t>Has X button</t>
+  </si>
+  <si>
+    <t>Has reject button on first div</t>
+  </si>
+  <si>
+    <t>Has reject button after pressing "select cookies"</t>
+  </si>
+  <si>
+    <t>Div "select cookies"</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>&lt;button class="mgbutton moove-gdpr-infobar-settings-btn change-settings-button gdpr-fbo-2" data-href="#moove_gdpr_cookie_modal" aria-label="Setari cookie-uri"&gt;Setari cookie-uri&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO (don't need it)</t>
+  </si>
+  <si>
+    <t>&lt;div id="onetrust-pc-btn-container"&gt;&lt;button id="onetrust-pc-btn-handler"&gt;Customize&lt;/button&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Div "reject" </t>
+  </si>
+  <si>
+    <t>Div "x"</t>
+  </si>
+  <si>
+    <t>&lt;div id="onetrust-reject-btn-container"&gt;&lt;button id="onetrust-reject-all-handler"&gt;Decline&lt;/button&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div id="onetrust-close-btn-container"&gt;&lt;button class="onetrust-close-btn-handler onetrust-close-btn-ui banner-close-button ot-close-icon" style="background-image: url(&amp;quot;https://cdn.cookielaw.org/logos/static/ot_close.svg&amp;quot;);" aria-label="Close"&gt;&lt;/button&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button class="mgbutton moove-gdpr-modal-reject-all button-visible" aria-label="Respinge tot"&gt;Respinge tot&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button mode="secondary" size="large" class=" css-1hy2vtq"&gt;&lt;span&gt;MAI MULTE OPȚIUNI&lt;/span&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button mode="link" size="small" class=" css-8rroe4"&gt;RESPINGERE TOTALĂ&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>&lt;button class="cmplz-btn cmplz-view-preferences"&gt;Setari cookie&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="politica-de-confidentialitate" id="rejectGDPR"&gt;Refuz&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button id="CybotCookiebotDialogBodyButtonDecline" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Respinge&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button id="CybotCookiebotDialogBodyLevelButtonCustomize" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Personalizează&lt;div class="CybotCookiebotDialogArrow"&gt;&lt;/div&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div id="cookiescript_close" tabindex="0" role="button" aria-label="Close"&gt;×&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>SEE NOTEPAD</t>
+  </si>
+  <si>
+    <t>&lt;a class="declineAllButtonLower" tabindex="0" role="button" style=""&gt;Decline All&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button mode="secondary" size="large" class=" css-17a6g85"&gt;&lt;span&gt;MORE OPTIONS&lt;/span&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button class="qc-cmp2-close-icon" aria-label="Disagree"&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button mode="link" size="small" class=" css-1sbgruk"&gt;REJECT ALL&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="/accept-policy/false" class="btn btn-outline-primary btn-lg"&gt;Nu sunt de acord&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button id="onetrust-reject-all-handler"&gt;Reject All&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button id="onetrust-pc-btn-handler" class="cookie-setting-link"&gt;Cookies verwalten&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>&lt;div class="customBtn-pYoje"&gt;Customise cookies&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://www.giantbomb.com/</t>
+  </si>
+  <si>
+    <t>https://www.makita.ro/</t>
+  </si>
+  <si>
+    <t>https://www.blitz.ro/cluj-napoca</t>
+  </si>
+  <si>
+    <t>&lt;button class="cookies__close icon icon-close" title="Close cookies"&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button id="onetrust-pc-btn-handler"&gt;Show Purposes&lt;/button&gt;</t>
   </si>
 </sst>
 </file>
@@ -144,13 +260,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,7 +624,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A3" sqref="A3:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +650,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -526,7 +661,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -537,7 +672,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -548,7 +683,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -559,7 +694,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -570,7 +705,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -587,7 +722,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -604,7 +739,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -621,7 +756,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -638,7 +773,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -655,7 +790,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -672,7 +807,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -711,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6537F556-4FCE-4387-B0A5-42EE745AE473}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +873,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -749,7 +884,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -760,7 +895,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -777,7 +912,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -788,7 +923,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -805,7 +940,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -822,7 +957,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -839,7 +974,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -856,7 +991,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -873,7 +1008,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -890,7 +1025,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
@@ -907,7 +1042,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
@@ -939,7 +1074,825 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28565BD3-7B10-42B8-B1E1-4B38A88F2ABA}">
+  <dimension ref="A2:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>2560</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>839</v>
+      </c>
+      <c r="E7">
+        <v>660</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1311</v>
+      </c>
+      <c r="E8">
+        <v>2560</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>235</v>
+      </c>
+      <c r="E9">
+        <v>2560</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>202</v>
+      </c>
+      <c r="E10">
+        <v>2560</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>226</v>
+      </c>
+      <c r="E13">
+        <v>2048</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>276</v>
+      </c>
+      <c r="E14">
+        <v>650</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>185</v>
+      </c>
+      <c r="E15">
+        <v>6208</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>124</v>
+      </c>
+      <c r="E16">
+        <v>2560</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>142</v>
+      </c>
+      <c r="E17">
+        <v>2560</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{3FD889F9-E04F-4E9A-98C6-2FBD7AB450F3}"/>
+    <hyperlink ref="B9" r:id="rId2" location="6468" xr:uid="{8E6DDABC-32A7-4A09-B264-8CE27702492B}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{4740DD9C-0A62-4378-9985-0278F3C11325}"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{61401D95-8289-4081-A9E9-3F268DFC6337}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{F945CD51-A1A3-48EE-9875-C2C2836CFD3A}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{FBEC72D5-AB01-476F-A6F9-4A6FBEABDD4F}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{244028C0-3EE7-44CB-A80D-8EEB6D1573B9}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{EF61F573-80CD-4F3F-ACED-C228C1448724}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{B1805D64-1BA7-41AB-A45D-57BE8A283593}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{1D52E5DC-2483-45F4-8D0C-F86D5A60EC05}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{F358104E-F988-4545-AE45-258587937FA3}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{A9E0C6DC-22E6-4FF8-BFF5-7353C266FE71}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD7C9C1-03D4-4A5C-B528-2ED33B136DEE}">
+  <dimension ref="A2:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>839</v>
+      </c>
+      <c r="E7">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1311</v>
+      </c>
+      <c r="E8">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>235</v>
+      </c>
+      <c r="E9">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>202</v>
+      </c>
+      <c r="E10">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>226</v>
+      </c>
+      <c r="E13">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>276</v>
+      </c>
+      <c r="E14">
+        <v>650</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{852FA85E-23A6-4AB6-9286-369A913845F3}"/>
+    <hyperlink ref="B9" r:id="rId2" location="6468" xr:uid="{151EA511-28F7-4B5B-B844-86E0AFF1ABE7}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{1AC53C69-A253-46BC-8931-BCEEA849422D}"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{F2D8815C-FBDE-4150-8931-CDA89D5FD83C}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{F3F4DFD5-E6EB-444F-ACAF-5150938C3213}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{D750FC2E-D200-4F80-ACFA-B8695D9C5511}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{F8BEB5D9-74CF-4146-8F2F-AFD3A8F49A97}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{5E83C3DB-8AF1-4390-88BC-C27820822C1B}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{F8B7455D-C1D9-449D-9C3F-0F27B37640AF}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{0A12B77D-07F9-44EB-A0DC-632F50C94A1B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -1166,15 +2119,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1184,6 +2128,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1198,14 +2150,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Stable version with Reject, X and Custom button
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BC9C12-7486-4A8B-A4DD-1B91250C92A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD93A220-72A9-47A6-82C4-B386893DCD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
   <si>
     <t>Page</t>
   </si>
@@ -110,9 +110,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>&lt;button class="mgbutton moove-gdpr-infobar-settings-btn change-settings-button gdpr-fbo-2" data-href="#moove_gdpr_cookie_modal" aria-label="Setari cookie-uri"&gt;Setari cookie-uri&lt;/button&gt;</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -128,15 +125,6 @@
     <t>Div "x"</t>
   </si>
   <si>
-    <t>&lt;div id="onetrust-reject-btn-container"&gt;&lt;button id="onetrust-reject-all-handler"&gt;Decline&lt;/button&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div id="onetrust-close-btn-container"&gt;&lt;button class="onetrust-close-btn-handler onetrust-close-btn-ui banner-close-button ot-close-icon" style="background-image: url(&amp;quot;https://cdn.cookielaw.org/logos/static/ot_close.svg&amp;quot;);" aria-label="Close"&gt;&lt;/button&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;button class="mgbutton moove-gdpr-modal-reject-all button-visible" aria-label="Respinge tot"&gt;Respinge tot&lt;/button&gt;</t>
-  </si>
-  <si>
     <t>&lt;button mode="secondary" size="large" class=" css-1hy2vtq"&gt;&lt;span&gt;MAI MULTE OPȚIUNI&lt;/span&gt;&lt;/button&gt;</t>
   </si>
   <si>
@@ -146,51 +134,21 @@
     <t>-</t>
   </si>
   <si>
-    <t>&lt;button class="cmplz-btn cmplz-view-preferences"&gt;Setari cookie&lt;/button&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="politica-de-confidentialitate" id="rejectGDPR"&gt;Refuz&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;button id="CybotCookiebotDialogBodyButtonDecline" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Respinge&lt;/button&gt;</t>
-  </si>
-  <si>
-    <t>&lt;button id="CybotCookiebotDialogBodyLevelButtonCustomize" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Personalizează&lt;div class="CybotCookiebotDialogArrow"&gt;&lt;/div&gt;&lt;/button&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div id="cookiescript_close" tabindex="0" role="button" aria-label="Close"&gt;×&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>SEE NOTEPAD</t>
   </si>
   <si>
-    <t>&lt;a class="declineAllButtonLower" tabindex="0" role="button" style=""&gt;Decline All&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;button mode="secondary" size="large" class=" css-17a6g85"&gt;&lt;span&gt;MORE OPTIONS&lt;/span&gt;&lt;/button&gt;</t>
   </si>
   <si>
-    <t>&lt;button class="qc-cmp2-close-icon" aria-label="Disagree"&gt;&lt;/button&gt;</t>
-  </si>
-  <si>
     <t>&lt;button mode="link" size="small" class=" css-1sbgruk"&gt;REJECT ALL&lt;/button&gt;</t>
   </si>
   <si>
     <t>&lt;a href="/accept-policy/false" class="btn btn-outline-primary btn-lg"&gt;Nu sunt de acord&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;button id="onetrust-reject-all-handler"&gt;Reject All&lt;/button&gt;</t>
-  </si>
-  <si>
-    <t>&lt;button id="onetrust-pc-btn-handler" class="cookie-setting-link"&gt;Cookies verwalten&lt;/button&gt;</t>
-  </si>
-  <si>
     <t>???</t>
   </si>
   <si>
-    <t>&lt;div class="customBtn-pYoje"&gt;Customise cookies&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>https://www.giantbomb.com/</t>
   </si>
   <si>
@@ -200,20 +158,420 @@
     <t>https://www.blitz.ro/cluj-napoca</t>
   </si>
   <si>
-    <t>&lt;button class="cookies__close icon icon-close" title="Close cookies"&gt;&lt;/button&gt;</t>
-  </si>
-  <si>
     <t>&lt;button id="onetrust-pc-btn-handler"&gt;Show Purposes&lt;/button&gt;</t>
   </si>
   <si>
     <t>https://www.onetrust.com/products/cookie-consent/</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div class="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Btn-pYoje"&gt;Customise cookies&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button id="onetrust-pc-btn-handler" class="cookie-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-link"&gt;Cookies verwalten&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button id="CybotCookiebotDialogBodyLevelButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ize" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Personalizează&lt;div class="CybotCookiebotDialogArrow"&gt;&lt;/div&gt;&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button class="cmplz-btn cmplz-view-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>preferences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;Setari cookie&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button class="mgbutton moove-gdpr-infobar-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-btn change-settings-button gdpr-fbo-2" data-href="#moove_gdpr_cookie_modal" aria-label="Setari cookie-uri"&gt;Setari cookie-uri&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button id="onetrust-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-all-handler"&gt;Reject All&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;a class="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>decline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AllButtonLower" tabindex="0" role="button" style=""&gt;Decline All&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button id="CybotCookiebotDialogBodyButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Decline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" class="CybotCookiebotDialogBodyButton" tabindex="0" lang="ro"&gt;Respinge&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;a href="politica-de-confidentialitate" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GDPR"&gt;Refuz&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div id="onetrust-reject-btn-container"&gt;&lt;button id="onetrust-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-all-handler"&gt;Decline&lt;/button&gt;&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button class="mgbutton moove-gdpr-modal-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-all button-visible" aria-label="Respinge tot"&gt;Respinge tot&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div id="cookiescript_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" tabindex="0" role="button" aria-label="Close"&gt;×&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div id="onetrust-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-btn-container"&gt;&lt;button class="onetrust-close-btn-handler onetrust-close-btn-ui banner-close-button ot-close-icon" style="background-image: url(&amp;quot;https://cdn.cookielaw.org/logos/static/ot_close.svg&amp;quot;);" aria-label="Close"&gt;&lt;/button&gt;&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button class="cookies__</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon icon-close" title="Close cookies"&gt;&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;div id="onetrust-pc-btn-container"&gt;&lt;button id="onetrust-pc-btn-handler"&gt;Adjust my preferences&lt;/button&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div class="ot-btn-subcntr"&gt;&lt;button class="ot-pc-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>refuse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-all-handler" tabindex="0"&gt;Accept only necessary&lt;/button&gt; &lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button class="qc-cmp2-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-icon" aria-label="Disagree"&gt;&lt;/button&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +583,27 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1082,7 +1461,7 @@
   <dimension ref="A2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,10 +1503,10 @@
         <v>21</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1144,22 +1523,22 @@
         <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1173,19 +1552,19 @@
         <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>46</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
@@ -1208,19 +1587,19 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="L5" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -1234,22 +1613,22 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -1272,19 +1651,19 @@
         <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
@@ -1304,19 +1683,19 @@
         <v>2560</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
@@ -1339,19 +1718,19 @@
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1374,19 +1753,19 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1418,13 +1797,13 @@
         <v>22</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -1450,16 +1829,16 @@
         <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
@@ -1479,22 +1858,22 @@
         <v>2048</v>
       </c>
       <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="K13" s="11" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
@@ -1520,16 +1899,16 @@
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1537,7 +1916,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1552,19 +1931,19 @@
         <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>46</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1572,7 +1951,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1593,13 +1972,13 @@
         <v>22</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1607,7 +1986,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1619,7 +1998,7 @@
         <v>2560</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -1628,21 +2007,48 @@
         <v>22</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>212</v>
+      </c>
+      <c r="E18">
+        <v>1920</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="12" t="s">
         <v>55</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1659,6 +2065,7 @@
     <hyperlink ref="B6" r:id="rId10" xr:uid="{1D52E5DC-2483-45F4-8D0C-F86D5A60EC05}"/>
     <hyperlink ref="B15" r:id="rId11" xr:uid="{F358104E-F988-4545-AE45-258587937FA3}"/>
     <hyperlink ref="B16" r:id="rId12" xr:uid="{A9E0C6DC-22E6-4FF8-BFF5-7353C266FE71}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{504BF50D-4044-46EF-BE2D-A70D225E4381}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1895,6 +2302,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -2121,15 +2537,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2139,6 +2546,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2153,14 +2568,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Stable version with fetching buttons
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD93A220-72A9-47A6-82C4-B386893DCD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ABAD3B-2F52-4D26-B01E-A6DBA139CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28565BD3-7B10-42B8-B1E1-4B38A88F2ABA}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2302,15 +2302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -2537,6 +2528,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2546,14 +2546,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2568,6 +2560,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Over-engineered version; TestPhase4 failed miserably
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ABAD3B-2F52-4D26-B01E-A6DBA139CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52205309-3AA6-49BB-9A6D-EAD9A69F0459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="3" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
     <sheet name="Testing phase 2" sheetId="3" r:id="rId2"/>
     <sheet name="Testing phase 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Testing phase 4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="58">
   <si>
     <t>Page</t>
   </si>
@@ -642,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -668,6 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1460,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28565BD3-7B10-42B8-B1E1-4B38A88F2ABA}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2073,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD7C9C1-03D4-4A5C-B528-2ED33B136DEE}">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2096,7 +2097,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -2107,7 +2108,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -2118,7 +2119,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2135,7 +2136,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2146,7 +2147,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2197,7 +2198,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2214,7 +2215,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2234,7 +2235,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2251,7 +2252,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2268,7 +2269,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -2282,26 +2283,103 @@
       </c>
       <c r="E14">
         <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>185</v>
+      </c>
+      <c r="E15">
+        <v>6208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>124</v>
+      </c>
+      <c r="E16">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>142</v>
+      </c>
+      <c r="E17">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>212</v>
+      </c>
+      <c r="E18">
+        <v>1920</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{852FA85E-23A6-4AB6-9286-369A913845F3}"/>
-    <hyperlink ref="B9" r:id="rId2" location="6468" xr:uid="{151EA511-28F7-4B5B-B844-86E0AFF1ABE7}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{1AC53C69-A253-46BC-8931-BCEEA849422D}"/>
-    <hyperlink ref="B11" r:id="rId4" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{F2D8815C-FBDE-4150-8931-CDA89D5FD83C}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{F3F4DFD5-E6EB-444F-ACAF-5150938C3213}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{F8B7455D-C1D9-449D-9C3F-0F27B37640AF}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{0A12B77D-07F9-44EB-A0DC-632F50C94A1B}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{5E83C3DB-8AF1-4390-88BC-C27820822C1B}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{F8BEB5D9-74CF-4146-8F2F-AFD3A8F49A97}"/>
     <hyperlink ref="B14" r:id="rId6" xr:uid="{D750FC2E-D200-4F80-ACFA-B8695D9C5511}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{F8BEB5D9-74CF-4146-8F2F-AFD3A8F49A97}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{5E83C3DB-8AF1-4390-88BC-C27820822C1B}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{F8B7455D-C1D9-449D-9C3F-0F27B37640AF}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{0A12B77D-07F9-44EB-A0DC-632F50C94A1B}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{F3F4DFD5-E6EB-444F-ACAF-5150938C3213}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{F2D8815C-FBDE-4150-8931-CDA89D5FD83C}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{1AC53C69-A253-46BC-8931-BCEEA849422D}"/>
+    <hyperlink ref="B9" r:id="rId10" location="6468" xr:uid="{151EA511-28F7-4B5B-B844-86E0AFF1ABE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -2528,15 +2606,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2546,6 +2615,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2560,14 +2637,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
A version with resize window that works
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52205309-3AA6-49BB-9A6D-EAD9A69F0459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA13D58E-926F-49D5-B14A-97C44BDEFEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="3" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="4" activeTab="5" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
     <sheet name="Testing phase 2" sheetId="3" r:id="rId2"/>
     <sheet name="Testing phase 3" sheetId="4" r:id="rId3"/>
     <sheet name="Testing phase 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Weight convention" sheetId="6" r:id="rId5"/>
+    <sheet name="Testing phase 5" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="79">
   <si>
     <t>Page</t>
   </si>
@@ -566,12 +568,75 @@
       <t>-icon" aria-label="Disagree"&gt;&lt;/button&gt;</t>
     </r>
   </si>
+  <si>
+    <t>BUTTON</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>CLASS</t>
+  </si>
+  <si>
+    <t>ARIA-LABEL</t>
+  </si>
+  <si>
+    <t>COOKIE/GDPR</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>WRAP</t>
+  </si>
+  <si>
+    <t>NO COOKIE/GDPR</t>
+  </si>
+  <si>
+    <t>NO ALL</t>
+  </si>
+  <si>
+    <t>NO WRAP</t>
+  </si>
+  <si>
+    <t>Finds the button for basket</t>
+  </si>
+  <si>
+    <t>Still 0 :))))</t>
+  </si>
+  <si>
+    <t>Gaseste doar butonul de customise</t>
+  </si>
+  <si>
+    <t>KO pt btonul de customise si close</t>
+  </si>
+  <si>
+    <t>Nu gaseste niciun buton</t>
+  </si>
+  <si>
+    <t>Gaseste tot &lt;3</t>
+  </si>
+  <si>
+    <t>Nu prea ok</t>
+  </si>
+  <si>
+    <t>KO pt butonul de close</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ok-ish</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,8 +673,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,6 +705,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -642,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -669,6 +752,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1461,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28565BD3-7B10-42B8-B1E1-4B38A88F2ABA}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F18"/>
+    <sheetView topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2076,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD7C9C1-03D4-4A5C-B528-2ED33B136DEE}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -2370,16 +2455,3349 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E574034-45C3-4C06-9CED-89EA761A56DB}">
+  <dimension ref="A2:U53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>-5</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6">
+        <f>$H$2</f>
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <f>$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N6">
+        <f>SUM(H6:L6)</f>
+        <v>54</v>
+      </c>
+      <c r="P6">
+        <v>59</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>60</v>
+      </c>
+      <c r="R6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" t="s">
+        <v>63</v>
+      </c>
+      <c r="T6" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H21" si="0">$H$2</f>
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I13" si="1">$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J9" si="2">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>SUM(H7:L7)</f>
+        <v>59</v>
+      </c>
+      <c r="P7">
+        <v>57</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N8">
+        <f>SUM(H8:L8)</f>
+        <v>52</v>
+      </c>
+      <c r="P8">
+        <v>56</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>60</v>
+      </c>
+      <c r="R8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" t="s">
+        <v>64</v>
+      </c>
+      <c r="U8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14">
+        <f>SUM(H9:L9)</f>
+        <v>57</v>
+      </c>
+      <c r="P9">
+        <v>54</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>60</v>
+      </c>
+      <c r="R9" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N10">
+        <f>SUM(H10:L10)</f>
+        <v>51</v>
+      </c>
+      <c r="P10">
+        <v>54</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T10" t="s">
+        <v>67</v>
+      </c>
+      <c r="U10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14">
+        <f>SUM(H11:L11)</f>
+        <v>56</v>
+      </c>
+      <c r="P11">
+        <v>52</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N12">
+        <f>SUM(H12:L12)</f>
+        <v>49</v>
+      </c>
+      <c r="P12">
+        <v>51</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" t="s">
+        <v>64</v>
+      </c>
+      <c r="U12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>SUM(H13:L13)</f>
+        <v>54</v>
+      </c>
+      <c r="P13">
+        <v>49</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" t="s">
+        <v>58</v>
+      </c>
+      <c r="S13" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <f>$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N14">
+        <f>SUM(H14:L14)</f>
+        <v>44</v>
+      </c>
+      <c r="P14">
+        <v>49</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>60</v>
+      </c>
+      <c r="R14" t="s">
+        <v>59</v>
+      </c>
+      <c r="S14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" t="s">
+        <v>64</v>
+      </c>
+      <c r="U14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I21" si="3">$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:J17" si="4">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>SUM(H15:L15)</f>
+        <v>49</v>
+      </c>
+      <c r="P15">
+        <v>49</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T15" t="s">
+        <v>64</v>
+      </c>
+      <c r="U15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N16">
+        <f>SUM(H16:L16)</f>
+        <v>42</v>
+      </c>
+      <c r="P16">
+        <v>47</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>60</v>
+      </c>
+      <c r="R16" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" t="s">
+        <v>63</v>
+      </c>
+      <c r="T16" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J17">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>SUM(H17:L17)</f>
+        <v>47</v>
+      </c>
+      <c r="P17">
+        <v>47</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R17" t="s">
+        <v>58</v>
+      </c>
+      <c r="S17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N18">
+        <f>SUM(H18:L18)</f>
+        <v>41</v>
+      </c>
+      <c r="P18">
+        <v>46</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" t="s">
+        <v>59</v>
+      </c>
+      <c r="S18" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" t="s">
+        <v>64</v>
+      </c>
+      <c r="U18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>SUM(H19:L19)</f>
+        <v>46</v>
+      </c>
+      <c r="P19">
+        <v>46</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>61</v>
+      </c>
+      <c r="R19" t="s">
+        <v>58</v>
+      </c>
+      <c r="S19" t="s">
+        <v>66</v>
+      </c>
+      <c r="T19" t="s">
+        <v>64</v>
+      </c>
+      <c r="U19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N20">
+        <f>SUM(H20:L20)</f>
+        <v>39</v>
+      </c>
+      <c r="P20">
+        <v>44</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>60</v>
+      </c>
+      <c r="R20" t="s">
+        <v>59</v>
+      </c>
+      <c r="S20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T20" t="s">
+        <v>64</v>
+      </c>
+      <c r="U20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>SUM(H21:L21)</f>
+        <v>44</v>
+      </c>
+      <c r="P21">
+        <v>44</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>60</v>
+      </c>
+      <c r="R21" t="s">
+        <v>59</v>
+      </c>
+      <c r="S21" t="s">
+        <v>66</v>
+      </c>
+      <c r="T21" t="s">
+        <v>67</v>
+      </c>
+      <c r="U21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22">
+        <f>$I$2</f>
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <f>$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N22">
+        <f>SUM(H22:L22)</f>
+        <v>44</v>
+      </c>
+      <c r="P22">
+        <v>44</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>61</v>
+      </c>
+      <c r="R22" t="s">
+        <v>58</v>
+      </c>
+      <c r="S22" t="s">
+        <v>63</v>
+      </c>
+      <c r="T22" t="s">
+        <v>64</v>
+      </c>
+      <c r="U22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H37" si="5">$I$2</f>
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I29" si="6">$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J25" si="7">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>SUM(H23:L23)</f>
+        <v>49</v>
+      </c>
+      <c r="P23">
+        <v>44</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>61</v>
+      </c>
+      <c r="R23" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" t="s">
+        <v>66</v>
+      </c>
+      <c r="T23" t="s">
+        <v>67</v>
+      </c>
+      <c r="U23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N24">
+        <f>SUM(H24:L24)</f>
+        <v>42</v>
+      </c>
+      <c r="P24">
+        <v>42</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>60</v>
+      </c>
+      <c r="R24" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" t="s">
+        <v>63</v>
+      </c>
+      <c r="T24" t="s">
+        <v>67</v>
+      </c>
+      <c r="U24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K25" s="14">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>SUM(H25:L25)</f>
+        <v>47</v>
+      </c>
+      <c r="P25">
+        <v>42</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>61</v>
+      </c>
+      <c r="R25" t="s">
+        <v>58</v>
+      </c>
+      <c r="S25" t="s">
+        <v>63</v>
+      </c>
+      <c r="T25" t="s">
+        <v>67</v>
+      </c>
+      <c r="U25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N26">
+        <f>SUM(H26:L26)</f>
+        <v>41</v>
+      </c>
+      <c r="P26">
+        <v>41</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>60</v>
+      </c>
+      <c r="R26" t="s">
+        <v>59</v>
+      </c>
+      <c r="S26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T26" t="s">
+        <v>64</v>
+      </c>
+      <c r="U26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L27" s="14">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>SUM(H27:L27)</f>
+        <v>46</v>
+      </c>
+      <c r="P27">
+        <v>41</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>61</v>
+      </c>
+      <c r="R27" t="s">
+        <v>58</v>
+      </c>
+      <c r="S27" t="s">
+        <v>66</v>
+      </c>
+      <c r="T27" t="s">
+        <v>64</v>
+      </c>
+      <c r="U27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N28">
+        <f>SUM(H28:L28)</f>
+        <v>39</v>
+      </c>
+      <c r="P28">
+        <v>39</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>60</v>
+      </c>
+      <c r="R28" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28" t="s">
+        <v>66</v>
+      </c>
+      <c r="T28" t="s">
+        <v>67</v>
+      </c>
+      <c r="U28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f>SUM(H29:L29)</f>
+        <v>44</v>
+      </c>
+      <c r="P29">
+        <v>39</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>61</v>
+      </c>
+      <c r="R29" t="s">
+        <v>58</v>
+      </c>
+      <c r="S29" t="s">
+        <v>66</v>
+      </c>
+      <c r="T29" t="s">
+        <v>67</v>
+      </c>
+      <c r="U29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I30">
+        <f>$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L30">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N30">
+        <f>SUM(H30:L30)</f>
+        <v>34</v>
+      </c>
+      <c r="P30">
+        <v>39</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>61</v>
+      </c>
+      <c r="R30" t="s">
+        <v>59</v>
+      </c>
+      <c r="S30" t="s">
+        <v>63</v>
+      </c>
+      <c r="T30" t="s">
+        <v>64</v>
+      </c>
+      <c r="U30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:I37" si="8">$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31:J33" si="9">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f>SUM(H31:L31)</f>
+        <v>39</v>
+      </c>
+      <c r="P31">
+        <v>39</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>62</v>
+      </c>
+      <c r="R31" t="s">
+        <v>58</v>
+      </c>
+      <c r="S31" t="s">
+        <v>63</v>
+      </c>
+      <c r="T31" t="s">
+        <v>64</v>
+      </c>
+      <c r="U31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N32">
+        <f>SUM(H32:L32)</f>
+        <v>32</v>
+      </c>
+      <c r="P32">
+        <v>37</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>61</v>
+      </c>
+      <c r="R32" t="s">
+        <v>59</v>
+      </c>
+      <c r="S32" t="s">
+        <v>63</v>
+      </c>
+      <c r="T32" t="s">
+        <v>67</v>
+      </c>
+      <c r="U32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f>SUM(H33:L33)</f>
+        <v>37</v>
+      </c>
+      <c r="P33">
+        <v>37</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>62</v>
+      </c>
+      <c r="R33" t="s">
+        <v>58</v>
+      </c>
+      <c r="S33" t="s">
+        <v>63</v>
+      </c>
+      <c r="T33" t="s">
+        <v>67</v>
+      </c>
+      <c r="U33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N34">
+        <f>SUM(H34:L34)</f>
+        <v>31</v>
+      </c>
+      <c r="P34">
+        <v>36</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>61</v>
+      </c>
+      <c r="R34" t="s">
+        <v>59</v>
+      </c>
+      <c r="S34" t="s">
+        <v>66</v>
+      </c>
+      <c r="T34" t="s">
+        <v>64</v>
+      </c>
+      <c r="U34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f>SUM(H35:L35)</f>
+        <v>36</v>
+      </c>
+      <c r="P35">
+        <v>36</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>62</v>
+      </c>
+      <c r="R35" t="s">
+        <v>58</v>
+      </c>
+      <c r="S35" t="s">
+        <v>66</v>
+      </c>
+      <c r="T35" t="s">
+        <v>64</v>
+      </c>
+      <c r="U35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N36">
+        <f>SUM(H36:L36)</f>
+        <v>29</v>
+      </c>
+      <c r="P36">
+        <v>34</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>61</v>
+      </c>
+      <c r="R36" t="s">
+        <v>59</v>
+      </c>
+      <c r="S36" t="s">
+        <v>63</v>
+      </c>
+      <c r="T36" t="s">
+        <v>64</v>
+      </c>
+      <c r="U36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f>SUM(H37:L37)</f>
+        <v>34</v>
+      </c>
+      <c r="P37">
+        <v>34</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>61</v>
+      </c>
+      <c r="R37" t="s">
+        <v>59</v>
+      </c>
+      <c r="S37" t="s">
+        <v>66</v>
+      </c>
+      <c r="T37" t="s">
+        <v>67</v>
+      </c>
+      <c r="U37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38">
+        <f>$H$3</f>
+        <v>10</v>
+      </c>
+      <c r="I38">
+        <f>$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K38">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N38">
+        <f>SUM(H38:L38)</f>
+        <v>34</v>
+      </c>
+      <c r="P38">
+        <v>34</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>62</v>
+      </c>
+      <c r="R38" t="s">
+        <v>58</v>
+      </c>
+      <c r="S38" t="s">
+        <v>63</v>
+      </c>
+      <c r="T38" t="s">
+        <v>64</v>
+      </c>
+      <c r="U38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39">
+        <f t="shared" ref="H39:H53" si="10">$H$3</f>
+        <v>10</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:I45" si="11">$J$2</f>
+        <v>24</v>
+      </c>
+      <c r="J39">
+        <f t="shared" ref="J39:J41" si="12">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f>SUM(H39:L39)</f>
+        <v>39</v>
+      </c>
+      <c r="P39">
+        <v>34</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>62</v>
+      </c>
+      <c r="R39" t="s">
+        <v>58</v>
+      </c>
+      <c r="S39" t="s">
+        <v>66</v>
+      </c>
+      <c r="T39" t="s">
+        <v>67</v>
+      </c>
+      <c r="U39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N40">
+        <f>SUM(H40:L40)</f>
+        <v>32</v>
+      </c>
+      <c r="P40">
+        <v>32</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>61</v>
+      </c>
+      <c r="R40" t="s">
+        <v>59</v>
+      </c>
+      <c r="S40" t="s">
+        <v>63</v>
+      </c>
+      <c r="T40" t="s">
+        <v>67</v>
+      </c>
+      <c r="U40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K41" s="14">
+        <v>0</v>
+      </c>
+      <c r="L41" s="14">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f>SUM(H41:L41)</f>
+        <v>37</v>
+      </c>
+      <c r="P41">
+        <v>32</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>62</v>
+      </c>
+      <c r="R41" t="s">
+        <v>58</v>
+      </c>
+      <c r="S41" t="s">
+        <v>63</v>
+      </c>
+      <c r="T41" t="s">
+        <v>67</v>
+      </c>
+      <c r="U41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N42">
+        <f>SUM(H42:L42)</f>
+        <v>31</v>
+      </c>
+      <c r="P42">
+        <v>31</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>61</v>
+      </c>
+      <c r="R42" t="s">
+        <v>59</v>
+      </c>
+      <c r="S42" t="s">
+        <v>66</v>
+      </c>
+      <c r="T42" t="s">
+        <v>64</v>
+      </c>
+      <c r="U42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L43" s="14">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <f>SUM(H43:L43)</f>
+        <v>36</v>
+      </c>
+      <c r="P43">
+        <v>31</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>62</v>
+      </c>
+      <c r="R43" t="s">
+        <v>58</v>
+      </c>
+      <c r="S43" t="s">
+        <v>66</v>
+      </c>
+      <c r="T43" t="s">
+        <v>64</v>
+      </c>
+      <c r="U43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N44">
+        <f>SUM(H44:L44)</f>
+        <v>29</v>
+      </c>
+      <c r="P44">
+        <v>29</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>61</v>
+      </c>
+      <c r="R44" t="s">
+        <v>59</v>
+      </c>
+      <c r="S44" t="s">
+        <v>66</v>
+      </c>
+      <c r="T44" t="s">
+        <v>67</v>
+      </c>
+      <c r="U44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f>SUM(H45:L45)</f>
+        <v>34</v>
+      </c>
+      <c r="P45">
+        <v>29</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>62</v>
+      </c>
+      <c r="R45" t="s">
+        <v>58</v>
+      </c>
+      <c r="S45" t="s">
+        <v>66</v>
+      </c>
+      <c r="T45" t="s">
+        <v>67</v>
+      </c>
+      <c r="U45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I46">
+        <f>$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J46">
+        <f>$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N46">
+        <f>SUM(H46:L46)</f>
+        <v>24</v>
+      </c>
+      <c r="P46">
+        <v>29</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>62</v>
+      </c>
+      <c r="R46" t="s">
+        <v>59</v>
+      </c>
+      <c r="S46" t="s">
+        <v>63</v>
+      </c>
+      <c r="T46" t="s">
+        <v>64</v>
+      </c>
+      <c r="U46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <f t="shared" ref="I47:I53" si="13">$K$2</f>
+        <v>14</v>
+      </c>
+      <c r="J47">
+        <f t="shared" ref="J47:J49" si="14">$L$2</f>
+        <v>3</v>
+      </c>
+      <c r="K47">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f>SUM(H47:L47)</f>
+        <v>29</v>
+      </c>
+      <c r="P47">
+        <v>27</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>62</v>
+      </c>
+      <c r="R47" t="s">
+        <v>59</v>
+      </c>
+      <c r="S47" t="s">
+        <v>63</v>
+      </c>
+      <c r="T47" t="s">
+        <v>67</v>
+      </c>
+      <c r="U47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N48">
+        <f>SUM(H48:L48)</f>
+        <v>22</v>
+      </c>
+      <c r="P48">
+        <v>26</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R48" t="s">
+        <v>59</v>
+      </c>
+      <c r="S48" t="s">
+        <v>66</v>
+      </c>
+      <c r="T48" t="s">
+        <v>64</v>
+      </c>
+      <c r="U48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <f>SUM(H49:L49)</f>
+        <v>27</v>
+      </c>
+      <c r="P49">
+        <v>24</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>62</v>
+      </c>
+      <c r="R49" t="s">
+        <v>59</v>
+      </c>
+      <c r="S49" t="s">
+        <v>63</v>
+      </c>
+      <c r="T49" t="s">
+        <v>64</v>
+      </c>
+      <c r="U49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N50">
+        <f>SUM(H50:L50)</f>
+        <v>21</v>
+      </c>
+      <c r="P50">
+        <v>24</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>62</v>
+      </c>
+      <c r="R50" t="s">
+        <v>59</v>
+      </c>
+      <c r="S50" t="s">
+        <v>66</v>
+      </c>
+      <c r="T50" t="s">
+        <v>67</v>
+      </c>
+      <c r="U50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <f>$M$2</f>
+        <v>2</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <f>SUM(H51:L51)</f>
+        <v>26</v>
+      </c>
+      <c r="P51">
+        <v>22</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>62</v>
+      </c>
+      <c r="R51" t="s">
+        <v>59</v>
+      </c>
+      <c r="S51" t="s">
+        <v>63</v>
+      </c>
+      <c r="T51" t="s">
+        <v>67</v>
+      </c>
+      <c r="U51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" t="s">
+        <v>65</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <f>$N$2</f>
+        <v>-5</v>
+      </c>
+      <c r="N52">
+        <f>SUM(H52:L52)</f>
+        <v>19</v>
+      </c>
+      <c r="P52">
+        <v>21</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>62</v>
+      </c>
+      <c r="R52" t="s">
+        <v>59</v>
+      </c>
+      <c r="S52" t="s">
+        <v>66</v>
+      </c>
+      <c r="T52" t="s">
+        <v>64</v>
+      </c>
+      <c r="U52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <f>SUM(H53:L53)</f>
+        <v>24</v>
+      </c>
+      <c r="P53">
+        <v>19</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>62</v>
+      </c>
+      <c r="R53" t="s">
+        <v>59</v>
+      </c>
+      <c r="S53" t="s">
+        <v>66</v>
+      </c>
+      <c r="T53" t="s">
+        <v>67</v>
+      </c>
+      <c r="U53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P6:U53">
+    <sortCondition descending="1" ref="P6:P53"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFFC5FE-73A0-40F3-B5E0-E7444F8510A2}">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>2560</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>839</v>
+      </c>
+      <c r="E7">
+        <v>660</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1311</v>
+      </c>
+      <c r="E8">
+        <v>2560</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>235</v>
+      </c>
+      <c r="E9">
+        <v>2560</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>202</v>
+      </c>
+      <c r="E10">
+        <v>2560</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>226</v>
+      </c>
+      <c r="E13">
+        <v>2048</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>276</v>
+      </c>
+      <c r="E14">
+        <v>650</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>185</v>
+      </c>
+      <c r="E15">
+        <v>6208</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>124</v>
+      </c>
+      <c r="E16">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>142</v>
+      </c>
+      <c r="E17">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>212</v>
+      </c>
+      <c r="E18">
+        <v>1920</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{2F14EF4F-FD14-4924-9CFB-8D6D0A8477AC}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{6CE447A7-31DC-47DC-9F49-35172321459F}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{5EBD8A39-63E1-49A8-A5AA-14CF76DF2838}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{AD370B34-AFBF-42C5-8132-8B99CA66F9FD}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{7DDC1765-C77C-4B67-B752-EC37E264D7A9}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{D30CD62D-C1B4-4A78-B7AD-6D425C554506}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{E598B071-279A-4D36-B05C-0E21856D51A0}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{F7F263FE-5943-49E9-91C9-7DAC28EDA519}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{918C3321-5ACC-4506-8D14-A562FE6EA0A4}"/>
+    <hyperlink ref="B9" r:id="rId10" location="6468" xr:uid="{6A134E39-A5F3-48B5-B6E8-BF3D3F4F80D2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -2606,6 +6024,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2615,14 +6042,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2637,6 +6056,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Version 2.0 (almost everything works) needs some small improvements
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA13D58E-926F-49D5-B14A-97C44BDEFEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4209F43-CA70-4BC7-B6C6-9D3DDAAB7978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="4" activeTab="5" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="6" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Testing phase 4" sheetId="5" r:id="rId4"/>
     <sheet name="Weight convention" sheetId="6" r:id="rId5"/>
     <sheet name="Testing phase 5" sheetId="7" r:id="rId6"/>
+    <sheet name="Testing phase 6" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="80">
   <si>
     <t>Page</t>
   </si>
@@ -630,6 +631,9 @@
   </si>
   <si>
     <t>ok-ish</t>
+  </si>
+  <si>
+    <t>Nope, look better</t>
   </si>
 </sst>
 </file>
@@ -725,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -754,6 +758,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2585,7 +2592,7 @@
         <v>-5</v>
       </c>
       <c r="N6">
-        <f>SUM(H6:L6)</f>
+        <f t="shared" ref="N6:N53" si="0">SUM(H6:L6)</f>
         <v>54</v>
       </c>
       <c r="P6">
@@ -2627,15 +2634,15 @@
         <v>68</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H21" si="0">$H$2</f>
+        <f t="shared" ref="H7:H21" si="1">$H$2</f>
         <v>30</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I13" si="1">$J$2</f>
+        <f t="shared" ref="I7:I13" si="2">$J$2</f>
         <v>24</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J9" si="2">$L$2</f>
+        <f t="shared" ref="J7:J9" si="3">$L$2</f>
         <v>3</v>
       </c>
       <c r="K7">
@@ -2646,7 +2653,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <f>SUM(H7:L7)</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="P7">
@@ -2688,15 +2695,15 @@
         <v>65</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="K8">
@@ -2707,7 +2714,7 @@
         <v>-5</v>
       </c>
       <c r="N8">
-        <f>SUM(H8:L8)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="P8">
@@ -2749,15 +2756,15 @@
         <v>68</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="K9" s="14">
@@ -2768,7 +2775,7 @@
       </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14">
-        <f>SUM(H9:L9)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="P9">
@@ -2810,11 +2817,11 @@
         <v>65</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J10">
@@ -2829,7 +2836,7 @@
         <v>-5</v>
       </c>
       <c r="N10">
-        <f>SUM(H10:L10)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="P10">
@@ -2871,11 +2878,11 @@
         <v>68</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J11" s="14">
@@ -2890,7 +2897,7 @@
       </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14">
-        <f>SUM(H11:L11)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="P11">
@@ -2932,11 +2939,11 @@
         <v>65</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J12">
@@ -2950,7 +2957,7 @@
         <v>-5</v>
       </c>
       <c r="N12">
-        <f>SUM(H12:L12)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="P12">
@@ -2992,24 +2999,24 @@
         <v>68</v>
       </c>
       <c r="H13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <f>SUM(H13:L13)</f>
         <v>54</v>
       </c>
       <c r="P13">
@@ -3051,7 +3058,7 @@
         <v>65</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I14">
@@ -3071,7 +3078,7 @@
         <v>-5</v>
       </c>
       <c r="N14">
-        <f>SUM(H14:L14)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="P14">
@@ -3113,15 +3120,15 @@
         <v>68</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:I21" si="3">$K$2</f>
+        <f t="shared" ref="I15:I21" si="4">$K$2</f>
         <v>14</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J17" si="4">$L$2</f>
+        <f t="shared" ref="J15:J16" si="5">$L$2</f>
         <v>3</v>
       </c>
       <c r="K15">
@@ -3132,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <f>SUM(H15:L15)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="P15">
@@ -3174,15 +3181,15 @@
         <v>65</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="K16">
@@ -3193,7 +3200,7 @@
         <v>-5</v>
       </c>
       <c r="N16">
-        <f>SUM(H16:L16)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="P16">
@@ -3235,11 +3242,11 @@
         <v>68</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J17">
@@ -3253,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <f>SUM(H17:L17)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="P17">
@@ -3295,11 +3302,11 @@
         <v>65</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J18">
@@ -3314,7 +3321,7 @@
         <v>-5</v>
       </c>
       <c r="N18">
-        <f>SUM(H18:L18)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="P18">
@@ -3356,11 +3363,11 @@
         <v>68</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J19">
@@ -3374,7 +3381,7 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <f>SUM(H19:L19)</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="P19">
@@ -3416,11 +3423,11 @@
         <v>65</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J20">
@@ -3434,7 +3441,7 @@
         <v>-5</v>
       </c>
       <c r="N20">
-        <f>SUM(H20:L20)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="P20">
@@ -3476,24 +3483,24 @@
         <v>68</v>
       </c>
       <c r="H21">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <f>SUM(H21:L21)</f>
         <v>44</v>
       </c>
       <c r="P21">
@@ -3555,7 +3562,7 @@
         <v>-5</v>
       </c>
       <c r="N22">
-        <f>SUM(H22:L22)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="P22">
@@ -3597,15 +3604,15 @@
         <v>68</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H37" si="5">$I$2</f>
+        <f t="shared" ref="H23:H37" si="6">$I$2</f>
         <v>20</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:I29" si="6">$J$2</f>
+        <f t="shared" ref="I23:I29" si="7">$J$2</f>
         <v>24</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:J25" si="7">$L$2</f>
+        <f t="shared" ref="J23:J25" si="8">$L$2</f>
         <v>3</v>
       </c>
       <c r="K23">
@@ -3616,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <f>SUM(H23:L23)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="P23">
@@ -3658,15 +3665,15 @@
         <v>65</v>
       </c>
       <c r="H24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="K24">
@@ -3677,7 +3684,7 @@
         <v>-5</v>
       </c>
       <c r="N24">
-        <f>SUM(H24:L24)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="P24">
@@ -3719,15 +3726,15 @@
         <v>68</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="K25" s="14">
@@ -3737,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <f>SUM(H25:L25)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="P25">
@@ -3779,11 +3786,11 @@
         <v>65</v>
       </c>
       <c r="H26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J26">
@@ -3798,7 +3805,7 @@
         <v>-5</v>
       </c>
       <c r="N26">
-        <f>SUM(H26:L26)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="P26">
@@ -3840,11 +3847,11 @@
         <v>68</v>
       </c>
       <c r="H27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J27">
@@ -3858,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <f>SUM(H27:L27)</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="P27">
@@ -3900,11 +3907,11 @@
         <v>65</v>
       </c>
       <c r="H28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J28">
@@ -3918,7 +3925,7 @@
         <v>-5</v>
       </c>
       <c r="N28">
-        <f>SUM(H28:L28)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="P28">
@@ -3960,11 +3967,11 @@
         <v>68</v>
       </c>
       <c r="H29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J29">
@@ -3977,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <f>SUM(H29:L29)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="P29">
@@ -4019,7 +4026,7 @@
         <v>65</v>
       </c>
       <c r="H30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I30">
@@ -4039,7 +4046,7 @@
         <v>-5</v>
       </c>
       <c r="N30">
-        <f>SUM(H30:L30)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="P30">
@@ -4081,15 +4088,15 @@
         <v>68</v>
       </c>
       <c r="H31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I37" si="8">$K$2</f>
+        <f t="shared" ref="I31:I37" si="9">$K$2</f>
         <v>14</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:J33" si="9">$L$2</f>
+        <f t="shared" ref="J31:J33" si="10">$L$2</f>
         <v>3</v>
       </c>
       <c r="K31">
@@ -4100,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="N31">
-        <f>SUM(H31:L31)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="P31">
@@ -4142,15 +4149,15 @@
         <v>65</v>
       </c>
       <c r="H32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="K32">
@@ -4161,7 +4168,7 @@
         <v>-5</v>
       </c>
       <c r="N32">
-        <f>SUM(H32:L32)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="P32">
@@ -4203,15 +4210,15 @@
         <v>68</v>
       </c>
       <c r="H33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="K33">
@@ -4221,7 +4228,7 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <f>SUM(H33:L33)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="P33">
@@ -4263,11 +4270,11 @@
         <v>65</v>
       </c>
       <c r="H34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J34">
@@ -4282,7 +4289,7 @@
         <v>-5</v>
       </c>
       <c r="N34">
-        <f>SUM(H34:L34)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="P34">
@@ -4324,11 +4331,11 @@
         <v>68</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J35">
@@ -4342,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <f>SUM(H35:L35)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="P35">
@@ -4384,11 +4391,11 @@
         <v>65</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J36">
@@ -4402,7 +4409,7 @@
         <v>-5</v>
       </c>
       <c r="N36">
-        <f>SUM(H36:L36)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="P36">
@@ -4444,11 +4451,11 @@
         <v>68</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="J37">
@@ -4461,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <f>SUM(H37:L37)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="P37">
@@ -4523,7 +4530,7 @@
         <v>-5</v>
       </c>
       <c r="N38">
-        <f>SUM(H38:L38)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="P38">
@@ -4565,15 +4572,15 @@
         <v>68</v>
       </c>
       <c r="H39">
-        <f t="shared" ref="H39:H53" si="10">$H$3</f>
+        <f t="shared" ref="H39:H53" si="11">$H$3</f>
         <v>10</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I45" si="11">$J$2</f>
+        <f t="shared" ref="I39:I45" si="12">$J$2</f>
         <v>24</v>
       </c>
       <c r="J39">
-        <f t="shared" ref="J39:J41" si="12">$L$2</f>
+        <f t="shared" ref="J39:J41" si="13">$L$2</f>
         <v>3</v>
       </c>
       <c r="K39">
@@ -4584,7 +4591,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <f>SUM(H39:L39)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="P39">
@@ -4626,15 +4633,15 @@
         <v>65</v>
       </c>
       <c r="H40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="K40">
@@ -4645,7 +4652,7 @@
         <v>-5</v>
       </c>
       <c r="N40">
-        <f>SUM(H40:L40)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="P40">
@@ -4687,15 +4694,15 @@
         <v>68</v>
       </c>
       <c r="H41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="K41" s="14">
@@ -4705,7 +4712,7 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <f>SUM(H41:L41)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="P41">
@@ -4747,11 +4754,11 @@
         <v>65</v>
       </c>
       <c r="H42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J42">
@@ -4766,7 +4773,7 @@
         <v>-5</v>
       </c>
       <c r="N42">
-        <f>SUM(H42:L42)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="P42">
@@ -4808,11 +4815,11 @@
         <v>68</v>
       </c>
       <c r="H43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J43">
@@ -4826,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <f>SUM(H43:L43)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="P43">
@@ -4868,11 +4875,11 @@
         <v>65</v>
       </c>
       <c r="H44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J44">
@@ -4886,7 +4893,7 @@
         <v>-5</v>
       </c>
       <c r="N44">
-        <f>SUM(H44:L44)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="P44">
@@ -4928,11 +4935,11 @@
         <v>68</v>
       </c>
       <c r="H45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="J45">
@@ -4945,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <f>SUM(H45:L45)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="P45">
@@ -4987,7 +4994,7 @@
         <v>65</v>
       </c>
       <c r="H46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I46">
@@ -5007,7 +5014,7 @@
         <v>-5</v>
       </c>
       <c r="N46">
-        <f>SUM(H46:L46)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="P46">
@@ -5049,15 +5056,15 @@
         <v>68</v>
       </c>
       <c r="H47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I47">
-        <f t="shared" ref="I47:I53" si="13">$K$2</f>
+        <f t="shared" ref="I47:I53" si="14">$K$2</f>
         <v>14</v>
       </c>
       <c r="J47">
-        <f t="shared" ref="J47:J49" si="14">$L$2</f>
+        <f t="shared" ref="J47:J49" si="15">$L$2</f>
         <v>3</v>
       </c>
       <c r="K47">
@@ -5068,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <f>SUM(H47:L47)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="P47">
@@ -5110,15 +5117,15 @@
         <v>65</v>
       </c>
       <c r="H48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="K48">
@@ -5129,7 +5136,7 @@
         <v>-5</v>
       </c>
       <c r="N48">
-        <f>SUM(H48:L48)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="P48">
@@ -5171,15 +5178,15 @@
         <v>68</v>
       </c>
       <c r="H49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="K49">
@@ -5189,7 +5196,7 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <f>SUM(H49:L49)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="P49">
@@ -5231,11 +5238,11 @@
         <v>65</v>
       </c>
       <c r="H50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J50">
@@ -5250,7 +5257,7 @@
         <v>-5</v>
       </c>
       <c r="N50">
-        <f>SUM(H50:L50)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="P50">
@@ -5292,11 +5299,11 @@
         <v>68</v>
       </c>
       <c r="H51">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J51">
@@ -5310,7 +5317,7 @@
         <v>0</v>
       </c>
       <c r="N51">
-        <f>SUM(H51:L51)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="P51">
@@ -5352,11 +5359,11 @@
         <v>65</v>
       </c>
       <c r="H52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J52">
@@ -5370,7 +5377,7 @@
         <v>-5</v>
       </c>
       <c r="N52">
-        <f>SUM(H52:L52)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="P52">
@@ -5412,11 +5419,11 @@
         <v>68</v>
       </c>
       <c r="H53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="I53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="J53">
@@ -5429,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <f>SUM(H53:L53)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="P53">
@@ -5463,8 +5470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFFC5FE-73A0-40F3-B5E0-E7444F8510A2}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="A17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5797,7 +5804,343 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540AF4F6-74FD-4A5F-BD00-45EED42BFFDE}">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="A18:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>76</v>
+      </c>
+      <c r="E5" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>839</v>
+      </c>
+      <c r="E7" s="14">
+        <v>660</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1311</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>235</v>
+      </c>
+      <c r="E9" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>202</v>
+      </c>
+      <c r="E10" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2560</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
+        <v>226</v>
+      </c>
+      <c r="E13" s="14">
+        <v>2048</v>
+      </c>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>276</v>
+      </c>
+      <c r="E14" s="14">
+        <v>650</v>
+      </c>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>185</v>
+      </c>
+      <c r="E15" s="14">
+        <v>6208</v>
+      </c>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14">
+        <v>124</v>
+      </c>
+      <c r="E16" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>142</v>
+      </c>
+      <c r="E17" s="14">
+        <v>2560</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>212</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1920</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.youdeal.ro/iasi" xr:uid="{A3614086-BA39-4A6F-9905-E366A61C4B4B}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{D09CD0FD-5130-4A27-9FB1-FA4EC2459ED8}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{07902D1D-1730-412E-A43C-18F6143D7ABF}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{4C45CC10-D5C9-4B25-83D0-3699D6F192E5}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{03D9E6F2-5EBA-4737-87C6-8C5B0572EA2B}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{8C8D6022-3F11-473D-9E4F-FED9B1811268}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{587C7E50-2104-4A8B-A8A1-6F0EBE1F5BD8}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://farmaciadedetergent.ro/product/cutiuta-cu-detergent-gel-proaspat-ca-marea-mireasma-din-tei/?utm_source=Facebook+Catalog+Feed+%2F+Instagram&amp;utm_campaign=FDD+Facebook+Catalogue+Feed&amp;utm_medium=cpc&amp;utm_term=626309&amp;utm_id=120200449959550606&amp;utm_content=120200449959540606&amp;fbclid=PAAaYqQuDNLTFIjC3-YRJ1mxu-D0a-pZbJCBK0zJB5Xbiv_XrU9d4NNbvENfU_aem_AXGlJoG_ah2GO-vCxQPdedrJg_kx05JfBWc3bhYueQmQw0jv-lkL2Bc3QXgabwOzPFI5LtPea9OIpqkaM1WomV4D" xr:uid="{467F5578-C62F-413B-90A2-B28FFF096359}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{62310D14-299D-4682-BCAA-55E2761DB624}"/>
+    <hyperlink ref="B9" r:id="rId10" location="6468" xr:uid="{3C784B39-8F0D-4805-865D-C894D2965DF3}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{80499550-1943-4D81-8DC4-DC912501B337}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a631a279-5a15-4d42-8c5c-c081a45901f6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -6024,24 +6367,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB8DB88-F110-4C4D-B0CC-7321E21A6D86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f8a1abd1-0732-4ba5-993c-eb9e15cff616"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a631a279-5a15-4d42-8c5c-c081a45901f6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6058,29 +6409,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB8DB88-F110-4C4D-B0CC-7321E21A6D86}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f8a1abd1-0732-4ba5-993c-eb9e15cff616"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final version before consulting with the coordinator
</commit_message>
<xml_diff>
--- a/TestPhases.xlsx
+++ b/TestPhases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dark-patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4209F43-CA70-4BC7-B6C6-9D3DDAAB7978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7B63FB-A5FE-4E64-BCCA-343543E04112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="6" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="2" xr2:uid="{29A26D87-942B-43B7-AD34-EE95EC441B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing phase 1" sheetId="1" r:id="rId1"/>
@@ -1553,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28565BD3-7B10-42B8-B1E1-4B38A88F2ABA}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5808,8 +5808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540AF4F6-74FD-4A5F-BD00-45EED42BFFDE}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="A18:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6132,15 +6132,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DAB8C56B376FAC4A84B43F14AF8279D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cee72c8f2d2b4d606a3a164027b3c8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a631a279-5a15-4d42-8c5c-c081a45901f6" xmlns:ns4="f8a1abd1-0732-4ba5-993c-eb9e15cff616" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86d72b4b6ab3434c81e3e9b67cbae157" ns3:_="" ns4:_="">
     <xsd:import namespace="a631a279-5a15-4d42-8c5c-c081a45901f6"/>
@@ -6367,6 +6358,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CB8DB88-F110-4C4D-B0CC-7321E21A6D86}">
   <ds:schemaRefs>
@@ -6385,14 +6385,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22EC23E3-2CF6-49FA-90C9-08A2E2EC9069}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6409,4 +6401,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A51DB4-3224-49AC-8EF0-BD000F5F88DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>